<commit_message>
got correct ways to measure curvuree usin ggeodesica and bsplines
</commit_message>
<xml_diff>
--- a/metadata/plate_metadata/20251017_part1_well_metadata.xlsx
+++ b/metadata/plate_metadata/20251017_part1_well_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marazzanocolon/Documents/PhD Folder/morphSeq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC28C1CC-F79B-2845-80A1-8087D09C7D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B579089A-FAD3-8B4D-87D4-32859703712D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20480" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20480" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="series_number_map" sheetId="7" r:id="rId7"/>
     <sheet name="start_age_morph" sheetId="8" r:id="rId8"/>
     <sheet name="embryos_per_well" sheetId="9" r:id="rId9"/>
-    <sheet name="temperature_c" sheetId="10" r:id="rId10"/>
+    <sheet name="temperature" sheetId="10" r:id="rId10"/>
     <sheet name="tricane" sheetId="12" r:id="rId11"/>
     <sheet name="notes" sheetId="13" r:id="rId12"/>
   </sheets>
@@ -1613,7 +1613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1316C8B-0927-DD44-AB74-6FEC17E4DB88}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>
@@ -3324,7 +3324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>

</xml_diff>